<commit_message>
Replaced TLV75201 by REG113NA 	modified:   "Bilan energ\303\251tique tracker GPS.xlsx" 	modified:   trackerGPS/microcontroller.bak 	modified:   trackerGPS/powerSupply.bak 	modified:   trackerGPS/powerSupply.sch 	modified:   trackerGPS/trackerGPS-cache.lib 	modified:   trackerGPS/trackerGPS.bak 	modified:   trackerGPS/trackerGPS.kicad_pcb 	modified:   trackerGPS/trackerGPS.kicad_pcb-bak 	modified:   trackerGPS/trackerGPS.sch
</commit_message>
<xml_diff>
--- a/Bilan energétique tracker GPS.xlsx
+++ b/Bilan energétique tracker GPS.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t>Modes de fonctionnement</t>
   </si>
@@ -156,6 +156,9 @@
   </si>
   <si>
     <t>LDO GPS</t>
+  </si>
+  <si>
+    <t>Vcc = Vbat + 225mV =3,925v</t>
   </si>
 </sst>
 </file>
@@ -1052,13 +1055,13 @@
   <dimension ref="B3:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="8" width="15.5703125"/>
@@ -1179,7 +1182,7 @@
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
added BOM and first prototype ready
</commit_message>
<xml_diff>
--- a/Bilan energétique tracker GPS.xlsx
+++ b/Bilan energétique tracker GPS.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="987" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Modes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Modes de fonctionnement</t>
   </si>
@@ -131,34 +131,49 @@
     <t>Pic de courant = 2A</t>
   </si>
   <si>
-    <t>Mode Actif : Module GSM en route, Module GPS réveille pendant 1 min en mode full power</t>
-  </si>
-  <si>
-    <t>Mode veille : Module GSM en route, Module GPS eteint pendant 4 min, MCU IDLE (Fsys = 1Mhz)</t>
-  </si>
-  <si>
     <t>Module GSM Quectel M95</t>
   </si>
   <si>
     <t>Module GPS Quectel L86</t>
   </si>
   <si>
-    <t xml:space="preserve">Mode reception SMS : </t>
-  </si>
-  <si>
     <t>LED</t>
   </si>
   <si>
-    <t>Vcc = 3,5v</t>
-  </si>
-  <si>
-    <t>LDO GSM UC</t>
-  </si>
-  <si>
     <t>LDO GPS</t>
   </si>
   <si>
     <t>Vcc = Vbat + 225mV =3,925v</t>
+  </si>
+  <si>
+    <t>LDO USB</t>
+  </si>
+  <si>
+    <t>Vcc = 3,3V</t>
+  </si>
+  <si>
+    <t>LDO  UC</t>
+  </si>
+  <si>
+    <t>CHARGER</t>
+  </si>
+  <si>
+    <t>Mode reception SMS : Module GSM en mode IDLE, MCU actif et GPS éteint.</t>
+  </si>
+  <si>
+    <t>1 mA.h = 3600 mA.s</t>
+  </si>
+  <si>
+    <t>Mode veille : Module GSM en route (SLEEP), Module GPS eteint pendant 4 min, MCU SLEEP (Fsys = 1Mhz)</t>
+  </si>
+  <si>
+    <t>Mode Actif : Module GSM en route (SLEEP), MCU actif, Module GPS réveille pendant 1 min en mode full power</t>
+  </si>
+  <si>
+    <t>12*4min / h</t>
+  </si>
+  <si>
+    <t>12*1min /h</t>
   </si>
 </sst>
 </file>
@@ -586,10 +601,10 @@
                 <c:formatCode>0.0%</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.16008269954958282</c:v>
+                  <c:v>0.22399222534216601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.83991730045041724</c:v>
+                  <c:v>0.77600777465783399</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -670,7 +685,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>779400</xdr:colOff>
+      <xdr:colOff>769875</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>157320</xdr:rowOff>
     </xdr:to>
@@ -960,14 +975,14 @@
   <dimension ref="B3:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="14.28515625"/>
-    <col min="3" max="3" width="90.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="98.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.28515625"/>
     <col min="5" max="5" width="21.7109375"/>
     <col min="6" max="1025" width="11.5703125"/>
@@ -1000,31 +1015,35 @@
         <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="D5" s="4">
         <v>69120</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="D6" s="4">
         <v>17280</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
@@ -1052,10 +1071,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I10"/>
+  <dimension ref="B3:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1064,11 +1083,14 @@
     <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="15.5703125"/>
-    <col min="9" max="1025" width="11.5703125"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="15.5703125"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="1027" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="20" t="s">
         <v>9</v>
       </c>
@@ -1079,34 +1101,42 @@
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+    </row>
+    <row r="4" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="str">
         <f>Modes!B5</f>
         <v>mode1</v>
@@ -1118,17 +1148,27 @@
         <v>0</v>
       </c>
       <c r="E5" s="9">
-        <v>0.8</v>
-      </c>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="10">
-        <f>SUM(C5:H5)</f>
-        <v>1300.8</v>
-      </c>
-    </row>
-    <row r="6" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+        <v>0.4</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>850</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="I5" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="10">
+        <f>SUM(C5:I5)</f>
+        <v>2150.4200000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="str">
         <f>Modes!B6</f>
         <v>mode2</v>
@@ -1139,16 +1179,28 @@
       <c r="D6" s="9">
         <v>26000</v>
       </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="10">
-        <f>SUM(C6:H6)</f>
-        <v>27300</v>
-      </c>
-    </row>
-    <row r="7" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="9">
+        <v>800</v>
+      </c>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>850</v>
+      </c>
+      <c r="H6" s="9">
+        <v>850</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.01</v>
+      </c>
+      <c r="J6" s="9"/>
+      <c r="K6" s="10">
+        <f>SUM(C6:I6)</f>
+        <v>29800.01</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="str">
         <f>Modes!B7</f>
         <v>mode3</v>
@@ -1159,12 +1211,14 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
-      <c r="I7" s="10">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10">
         <f>SUM(C7:H7)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="str">
         <f>Modes!B8</f>
         <v>mode4</v>
@@ -1175,14 +1229,16 @@
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
-      <c r="I8" s="10">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="10">
         <f>SUM(C8:H8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>31</v>
@@ -1191,14 +1247,14 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B3:K3"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <headerFooter>
@@ -1210,16 +1266,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B42:I48"/>
+  <dimension ref="B42:I51"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="11.5703125"/>
-    <col min="3" max="3" width="16.7109375"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="31.28515625"/>
     <col min="5" max="5" width="19.28515625"/>
     <col min="6" max="1025" width="11.5703125"/>
@@ -1264,16 +1320,16 @@
         <v>69120</v>
       </c>
       <c r="D44" s="9">
-        <f>'Conso inst'!I5</f>
-        <v>1300.8</v>
+        <f>'Conso inst'!K5</f>
+        <v>2150.4200000000005</v>
       </c>
       <c r="E44" s="13">
         <f>C44*D44/(3600*1000)</f>
-        <v>24.975359999999998</v>
+        <v>41.288064000000013</v>
       </c>
       <c r="F44" s="14">
         <f>E44/E48</f>
-        <v>0.16008269954958282</v>
+        <v>0.22399222534216601</v>
       </c>
     </row>
     <row r="45" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1286,16 +1342,16 @@
         <v>17280</v>
       </c>
       <c r="D45" s="9">
-        <f>'Conso inst'!I6</f>
-        <v>27300</v>
+        <f>'Conso inst'!K6</f>
+        <v>29800.01</v>
       </c>
       <c r="E45" s="13">
         <f>C45*D45/(3600*1000)</f>
-        <v>131.04</v>
+        <v>143.04004799999998</v>
       </c>
       <c r="F45" s="14">
         <f>E45/E48</f>
-        <v>0.83991730045041724</v>
+        <v>0.77600777465783399</v>
       </c>
     </row>
     <row r="46" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -1308,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="9">
-        <f>'Conso inst'!I7</f>
+        <f>'Conso inst'!K7</f>
         <v>0</v>
       </c>
       <c r="E46" s="13">
@@ -1330,7 +1386,7 @@
         <v>0</v>
       </c>
       <c r="D47" s="9">
-        <f>'Conso inst'!I8</f>
+        <f>'Conso inst'!K8</f>
         <v>0</v>
       </c>
       <c r="E47" s="13">
@@ -1350,11 +1406,16 @@
       <c r="D48" s="21"/>
       <c r="E48" s="13">
         <f>SUM(E44:E47)</f>
-        <v>156.01535999999999</v>
+        <v>184.328112</v>
       </c>
       <c r="F48" s="14">
         <f>E48/E48</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1376,7 +1437,7 @@
   <dimension ref="C2:F14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1501,7 +1562,7 @@
       <c r="E13" s="16"/>
       <c r="F13" s="9">
         <f>'Bilan energetique'!E48</f>
-        <v>156.01535999999999</v>
+        <v>184.328112</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>